<commit_message>
Added Ambient check and master loop. need to add the seperate curves
</commit_message>
<xml_diff>
--- a/data/Temp Curve Wksht.xlsx
+++ b/data/Temp Curve Wksht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\r720-fanspeed\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{271A7461-C657-4632-BA68-5E4F2E261E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1613E9A2-C5AE-45B3-A0F8-0ADCEAA6BEF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C3F76B91-CA7F-4F32-9702-10622C1027C3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C3F76B91-CA7F-4F32-9702-10622C1027C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Base Idle Temps" sheetId="1" r:id="rId1"/>
@@ -1470,16 +1470,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>428626</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>552449</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1806,9 +1806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D3DAF6-A91F-4358-A10A-496E74ABE7B2}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S26" sqref="S26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>